<commit_message>
not sure about publish and show user ads
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SoftUni\AngularJS\free-ads.ml\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +245,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -347,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -396,10 +403,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,11 +760,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -900,7 +910,7 @@
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="22">
         <v>5</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -912,7 +922,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="22">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1228,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>